<commit_message>
#35257 modify budzik boards
</commit_message>
<xml_diff>
--- a/pisak/res/external/zadanie/conditions.xlsx
+++ b/pisak/res/external/zadanie/conditions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jan/psychopy_budzik/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jan/pisak/pisak/res/external/zadanie/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21040" tabRatio="500"/>
+    <workbookView xWindow="9600" yWindow="440" windowWidth="19200" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>correct</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>object2</t>
+  </si>
+  <si>
+    <t>mała kaczka</t>
+  </si>
+  <si>
+    <t>duża kaczka</t>
   </si>
 </sst>
 </file>
@@ -359,7 +365,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
@@ -400,6 +406,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
#36225 translate object names to polish
</commit_message>
<xml_diff>
--- a/pisak/res/external/zadanie/conditions.xlsx
+++ b/pisak/res/external/zadanie/conditions.xlsx
@@ -32,15 +32,6 @@
     <t>correct</t>
   </si>
   <si>
-    <t>circle</t>
-  </si>
-  <si>
-    <t>square</t>
-  </si>
-  <si>
-    <t>triangle</t>
-  </si>
-  <si>
     <t>object1</t>
   </si>
   <si>
@@ -51,6 +42,15 @@
   </si>
   <si>
     <t>duża kaczka</t>
+  </si>
+  <si>
+    <t>koło</t>
+  </si>
+  <si>
+    <t>kwadrat</t>
+  </si>
+  <si>
+    <t>trójkąt</t>
   </si>
 </sst>
 </file>
@@ -368,17 +368,17 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -386,35 +386,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>